<commit_message>
make it full  better3
</commit_message>
<xml_diff>
--- a/public/TestFile/Registration_data_templete.xlsx
+++ b/public/TestFile/Registration_data_templete.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ezzowali/Desktop/Desktop/SMAV/smavacadmey/public/TestFile/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talbi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE74B698-C06B-EA4D-AC10-57B84F41FEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A176E82C-AED6-4A41-9AAF-62D67F2D6652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{E396899E-7DCE-9343-8E7A-425EC50BF2D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E396899E-7DCE-9343-8E7A-425EC50BF2D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,27 +39,12 @@
     <t xml:space="preserve">First name </t>
   </si>
   <si>
-    <t>middle name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">email </t>
-  </si>
-  <si>
-    <t xml:space="preserve">phone </t>
-  </si>
-  <si>
     <t xml:space="preserve">Education level </t>
   </si>
   <si>
     <t>age</t>
   </si>
   <si>
-    <t>Male or Female</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -190,17 +175,32 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>Middle name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone </t>
+  </si>
+  <si>
+    <t>Sex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -208,7 +208,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -218,16 +218,30 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -235,11 +249,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,9 +280,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="عادي" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -269,7 +305,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="نسق Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -565,250 +601,997 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB8847F-167C-784A-939F-C7DAE7C46907}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="5" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="K1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="O8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="O9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="O11" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="O12" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="O13" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="O14" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="O15" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="O16" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="O17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="O18" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="O19" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="O20" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="O21" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="O22" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="O23" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="O24" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="O25" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="O26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="O28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="O29" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="O30" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="O31" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="O32" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="O33" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="O34" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="O35" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="O36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="O37" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="O38" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="O39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="O40" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="O41" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="O42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="O44" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="O45" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="O46" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="O47" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="O48" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="O49" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="O50" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O52" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O53" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O54" s="4">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O55" s="4">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O56" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O57" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O58" s="4">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O59" s="4">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O60" s="4">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="F2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="1" t="s">
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O61" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="1" t="s">
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O62" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M10" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="H16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H17" s="1" t="s">
-        <v>29</v>
-      </c>
     </row>
   </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F53" xr:uid="{B4A31D11-7D00-4309-A9D0-D0A94E7F3329}">
+      <formula1>$O$8:$O$9</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H57" xr:uid="{88627E2B-7549-4A9A-9E44-1176168F4AB0}">
+      <formula1>$O$11:$O$26</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J44" xr:uid="{E86B5140-6D3A-40CA-B546-D382CEE74FD5}">
+      <formula1>$O$28:$O$42</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K56" xr:uid="{07D7FE00-872F-4BB4-A42B-48B8AA25060B}">
+      <formula1>$O$44:$O$50</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M58" xr:uid="{6D19560F-A54C-4603-9880-4D9F93AD30D8}">
+      <formula1>$O$52:$O$62</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>